<commit_message>
added datatype specific return method
</commit_message>
<xml_diff>
--- a/src/test/resources/files/simple_excle.xlsx
+++ b/src/test/resources/files/simple_excle.xlsx
@@ -20,9 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Test1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_col2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_col3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_col21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_col31</t>
   </si>
 </sst>
 </file>
@@ -234,10 +255,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:C3"/>
+  <dimension ref="A3:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -252,6 +273,39 @@
       <c r="C3" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add functionality for table reading
</commit_message>
<xml_diff>
--- a/src/test/resources/files/simple_excle.xlsx
+++ b/src/test/resources/files/simple_excle.xlsx
@@ -50,9 +50,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -128,7 +127,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -258,7 +257,7 @@
   <dimension ref="A3:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -271,8 +270,8 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">0</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
re organize , added spring boot sample
</commit_message>
<xml_diff>
--- a/src/test/resources/files/simple_excle.xlsx
+++ b/src/test/resources/files/simple_excle.xlsx
@@ -50,8 +50,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -127,7 +128,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -257,7 +258,7 @@
   <dimension ref="A3:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -269,41 +270,43 @@
       <c r="B3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+      <c r="C3" s="0" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>